<commit_message>
Added named queries for invasive / threatened species
</commit_message>
<xml_diff>
--- a/src/test/Nov30/Timor_Leste-November30.xlsx
+++ b/src/test/Nov30/Timor_Leste-November30.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SPECIES_INFORMATION" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">DESIGNATED_AREAS!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SPECIES_INFORMATION!$A$1:$Q$596</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SPECIES_INFORMATION!$A$1:$Q$597</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SPECIES_LOCATION!$A$1:$K$604</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10142" uniqueCount="2603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10147" uniqueCount="2607">
   <si>
     <t>KINGDOM</t>
   </si>
@@ -7837,6 +7837,18 @@
   </si>
   <si>
     <t>Ray finned fish</t>
+  </si>
+  <si>
+    <t>http://www.gbif.org/species/2347811</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Marine/Freshwater</t>
+  </si>
+  <si>
+    <t>Nino Konis Santana</t>
   </si>
 </sst>
 </file>
@@ -7846,7 +7858,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7959,6 +7971,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -7995,10 +8015,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8087,8 +8108,10 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8391,11 +8414,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O596"/>
+  <dimension ref="A1:O597"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A577" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E596" sqref="E596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -35447,29 +35470,49 @@
       <c r="A596" s="21" t="s">
         <v>2535</v>
       </c>
-      <c r="B596" s="16" t="s">
+      <c r="B596" s="30" t="s">
+        <v>2603</v>
+      </c>
+      <c r="J596" s="27" t="s">
+        <v>2548</v>
+      </c>
+      <c r="N596" s="21" t="s">
+        <v>2604</v>
+      </c>
+      <c r="O596" s="21" t="s">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="597" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A597" s="21" t="s">
+        <v>2535</v>
+      </c>
+      <c r="B597" s="16" t="s">
         <v>2590</v>
       </c>
-      <c r="J596" s="27" t="s">
+      <c r="J597" s="27" t="s">
         <v>2565</v>
       </c>
-      <c r="K596" s="21" t="s">
+      <c r="K597" s="21" t="s">
         <v>2591</v>
       </c>
-      <c r="N596" s="21" t="s">
+      <c r="N597" s="21" t="s">
         <v>2449</v>
       </c>
-      <c r="O596" s="21" t="s">
+      <c r="O597" s="21" t="s">
         <v>1225</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q596"/>
+  <autoFilter ref="A1:Q597"/>
   <sortState ref="A2:P599">
     <sortCondition ref="E2:E599"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B596" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -42259,7 +42302,7 @@
   <dimension ref="A1:XEW1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -58684,16 +58727,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="4"/>
+    <col min="1" max="1" width="33" style="4" customWidth="1"/>
     <col min="2" max="2" width="94.7109375" style="2" customWidth="1"/>
     <col min="3" max="16384" width="24.7109375" style="2"/>
   </cols>
@@ -58740,7 +58783,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2526</v>
       </c>
@@ -58748,7 +58791,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>2526</v>
       </c>
@@ -58757,7 +58800,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>2526</v>
       </c>
@@ -58767,7 +58810,7 @@
     </row>
     <row r="9" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>2457</v>
+        <v>2606</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2551</v>
@@ -58775,7 +58818,7 @@
     </row>
     <row r="10" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>2457</v>
+        <v>2606</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2598</v>
@@ -58784,7 +58827,7 @@
     </row>
     <row r="11" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>2457</v>
+        <v>2606</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2600</v>
@@ -58793,7 +58836,7 @@
     </row>
     <row r="12" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>2457</v>
+        <v>2606</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2597</v>
@@ -58802,15 +58845,15 @@
     </row>
     <row r="13" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>2457</v>
+        <v>2606</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2599</v>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="25" spans="2:2" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="24" spans="2:2" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>2559</v>
       </c>
     </row>
@@ -58922,8 +58965,8 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>